<commit_message>
splitsize test adjusted for clarity
</commit_message>
<xml_diff>
--- a/climateChangeData/climateChangeRes/ResultsData.xlsx
+++ b/climateChangeData/climateChangeRes/ResultsData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karth\Desktop\Karthik\Python_Projects\biaswrappersTest\climateChangeData\climateChangeRes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB92E3AF-A709-4F84-B214-8DF9DA3CD844}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC2DAE7-9903-4773-82F6-9A0D29AC7E94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SplitsizeRes" sheetId="1" r:id="rId1"/>
@@ -42,9 +42,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0.000000000"/>
-    <numFmt numFmtId="168" formatCode="#,##0.000000"/>
+    <numFmt numFmtId="165" formatCode="#,##0.000000"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -99,9 +100,6 @@
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -117,10 +115,13 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -428,174 +429,104 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.21875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
-        <v>0</v>
-      </c>
-      <c r="B2" s="8">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="B2" s="7">
+        <v>0.33304359399287697</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="B3" s="7">
+        <v>0.43059415405408902</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="11">
+        <v>0.3</v>
+      </c>
+      <c r="B4" s="7">
+        <v>0.20591644014812399</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="11">
+        <v>0.4</v>
+      </c>
+      <c r="B5" s="7">
+        <v>0.466553105681562</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="B6" s="7">
+        <v>1.0998256779753399</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="11">
+        <v>0.6</v>
+      </c>
+      <c r="B7" s="7">
+        <v>0.78664485712327004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="11">
+        <v>0.7</v>
+      </c>
+      <c r="B8" s="7">
+        <v>0.47502709351266997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="11">
+        <v>0.8</v>
+      </c>
+      <c r="B9" s="7">
+        <v>0.27446223947463599</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="11">
+        <v>0.9</v>
+      </c>
+      <c r="B10" s="7">
+        <v>0.98091787353330995</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="11">
+        <v>1</v>
+      </c>
+      <c r="B11" s="7">
         <v>0.37656558733025802</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="B3" s="8">
-        <v>0.33304359399287697</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
-        <v>0.15</v>
-      </c>
-      <c r="B4" s="8">
-        <v>0.30411610748369899</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="B5" s="8">
-        <v>0.43059415405408902</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
-        <v>0.25</v>
-      </c>
-      <c r="B6" s="8">
-        <v>0.27269466264939801</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="B7" s="8">
-        <v>0.20591644014812399</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="4">
-        <v>0.35</v>
-      </c>
-      <c r="B8" s="8">
-        <v>1.1142667586851001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="B9" s="8">
-        <v>0.466553105681562</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="4">
-        <v>0.45</v>
-      </c>
-      <c r="B10" s="8">
-        <v>0.75046707922685296</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="B11" s="8">
-        <v>1.0998256779753399</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="4">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="B12" s="8">
-        <v>0.77278133041419905</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="4">
-        <v>0.6</v>
-      </c>
-      <c r="B13" s="8">
-        <v>0.78664485712327004</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="4">
-        <v>0.65</v>
-      </c>
-      <c r="B14" s="8">
-        <v>0.474831830884059</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="B15" s="8">
-        <v>0.47502709351266997</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="4">
-        <v>0.75</v>
-      </c>
-      <c r="B16" s="8">
-        <v>0.37624519733942902</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="4">
-        <v>0.8</v>
-      </c>
-      <c r="B17" s="8">
-        <v>0.27446223947463599</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="4">
-        <v>0.85</v>
-      </c>
-      <c r="B18" s="8">
-        <v>0.30834111413396698</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="4">
-        <v>0.9</v>
-      </c>
-      <c r="B19" s="8">
-        <v>0.98091787353330995</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="4">
-        <v>0.95</v>
-      </c>
-      <c r="B20" s="8">
-        <v>0.69451938129678603</v>
       </c>
     </row>
   </sheetData>
@@ -610,14 +541,14 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B39" sqref="B39:B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="8.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.5546875" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -635,10 +566,10 @@
       <c r="A2" s="3">
         <v>0</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="9">
         <v>0.41203779263974899</v>
       </c>
-      <c r="C2" s="10">
+      <c r="C2" s="9">
         <v>0.170370970221288</v>
       </c>
     </row>
@@ -646,10 +577,10 @@
       <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="9">
         <v>0.34508119421512201</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="9">
         <v>0.17466039275839801</v>
       </c>
     </row>
@@ -657,21 +588,21 @@
       <c r="A4" s="3">
         <v>5</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="9">
         <v>0.29051077741003001</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="9">
         <v>0.17184889732536399</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>20</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="10">
         <v>0.63195997404948501</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="10">
         <v>0.166709010805555</v>
       </c>
     </row>

</xml_diff>